<commit_message>
3 FLUJOS NUEVOS SANITY
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/MovistarFija.xlsx
+++ b/src/main/resources/excel/MovistarFija.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
   <si>
     <t>TC1</t>
   </si>
@@ -130,13 +130,29 @@
   </si>
   <si>
     <t>04074425</t>
+  </si>
+  <si>
+    <t>PAQUETE HOGAR DIGITAL</t>
+  </si>
+  <si>
+    <t>MONO</t>
+  </si>
+  <si>
+    <t>TRÍO</t>
+  </si>
+  <si>
+    <t>TRIO PLANO LOCAL 200 MBPS ESTANDAR DIGITAL HD</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +175,21 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,36 +209,42 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="11">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hipervínculo" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -224,10 +261,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -262,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -297,7 +334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -391,21 +428,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -422,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -474,42 +511,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -596,7 +633,7 @@
       <c r="AN1" s="3"/>
       <c r="AO1" s="3"/>
     </row>
-    <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B2" s="5">
         <v>129431</v>
       </c>
@@ -646,13 +683,13 @@
         <v>26</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>33</v>
@@ -661,7 +698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>129431</v>
       </c>
@@ -726,88 +763,153 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="4" s="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>129431</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="6" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="7" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="8" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="9" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="10" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="11" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="12" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="13" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="14" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="15" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="16" s="1" spans="1:41" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="17" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="18" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="19" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="20" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="21" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="22" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="23" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="24" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="25" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="26" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="27" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="28" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="29" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="30" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="31" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="32" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="33" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="34" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="35" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="36" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="37" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="38" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="39" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="40" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="41" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="42" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="43" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="44" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="45" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="46" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="47" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="48" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="49" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="50" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="51" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="52" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="53" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="54" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="55" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="56" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="57" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="58" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="59" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="60" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="61" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="62" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="63" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="64" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="65" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="66" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="67" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="68" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="69" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="70" s="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="71" s="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D4" type="list">
       <formula1>"DNI,Carné de Extranjeria,Pasaporte,RUC,Otros Extranjeros - Aut. SNM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="R2:R4" type="list">
       <formula1>"TRÍO, DÚO,MONO"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId4" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>